<commit_message>
add new check and toast v-1
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK\Documents\Netology\QA\HW\Mod12_Diplom_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1796D52E-9506-441A-84E9-941793FC1645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF2770E-6D48-4B0B-B023-2977574E3CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="125">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -890,6 +890,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -904,54 +952,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1247,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,92 +1262,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="29">
+      <c r="B3" s="42"/>
+      <c r="C3" s="45">
         <v>45931</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="43"/>
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="33"/>
+      <c r="F6" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="34"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="40"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1363,7 +1363,7 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="5" t="s">
         <v>89</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="12" t="s">
         <v>90</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1431,7 +1431,7 @@
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="12" t="s">
         <v>16</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1471,11 +1471,13 @@
       <c r="D16" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="5" t="s">
         <v>84</v>
       </c>
@@ -1489,7 +1491,7 @@
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="43"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="12" t="s">
         <v>85</v>
       </c>
@@ -1503,7 +1505,7 @@
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1519,7 +1521,7 @@
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="5" t="s">
         <v>81</v>
       </c>
@@ -1533,7 +1535,7 @@
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="5" t="s">
         <v>86</v>
       </c>
@@ -1547,7 +1549,7 @@
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="43"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="12" t="s">
         <v>20</v>
       </c>
@@ -1561,7 +1563,7 @@
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1579,7 +1581,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="45"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="5" t="s">
         <v>91</v>
       </c>
@@ -1595,7 +1597,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="45"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="5" t="s">
         <v>92</v>
       </c>
@@ -1609,7 +1611,7 @@
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="45"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
         <v>93</v>
       </c>
@@ -1623,7 +1625,7 @@
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="45"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="5" t="s">
         <v>94</v>
       </c>
@@ -1637,7 +1639,7 @@
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="45"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="5" t="s">
         <v>95</v>
       </c>
@@ -1651,7 +1653,7 @@
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="46"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="12" t="s">
         <v>96</v>
       </c>
@@ -1665,7 +1667,7 @@
       <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -1681,7 +1683,7 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="45"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="5" t="s">
         <v>34</v>
       </c>
@@ -1695,7 +1697,7 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="5" t="s">
         <v>100</v>
       </c>
@@ -1711,7 +1713,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="46"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -1719,7 +1721,7 @@
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1735,7 +1737,7 @@
       <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="23" t="s">
         <v>114</v>
       </c>
@@ -1749,7 +1751,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="42"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="5" t="s">
         <v>103</v>
       </c>
@@ -1763,7 +1765,7 @@
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="5" t="s">
         <v>101</v>
       </c>
@@ -1777,7 +1779,7 @@
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="5" t="s">
         <v>102</v>
       </c>
@@ -1793,7 +1795,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="43"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="12" t="s">
         <v>104</v>
       </c>
@@ -1809,7 +1811,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="29" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -1825,7 +1827,7 @@
       <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="42"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="5" t="s">
         <v>39</v>
       </c>
@@ -1839,7 +1841,7 @@
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="42"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="5" t="s">
         <v>40</v>
       </c>
@@ -1853,7 +1855,7 @@
       <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="42"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="5" t="s">
         <v>121</v>
       </c>
@@ -1867,7 +1869,7 @@
       <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="42"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="5" t="s">
         <v>122</v>
       </c>
@@ -1881,7 +1883,7 @@
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="42"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="5" t="s">
         <v>41</v>
       </c>
@@ -1895,7 +1897,7 @@
       <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="42"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="5" t="s">
         <v>42</v>
       </c>
@@ -1909,7 +1911,7 @@
       <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="42"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="5" t="s">
         <v>123</v>
       </c>
@@ -1925,7 +1927,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="42"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="5" t="s">
         <v>43</v>
       </c>
@@ -1939,7 +1941,7 @@
       <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="43"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="12" t="s">
         <v>124</v>
       </c>
@@ -1955,7 +1957,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="29" t="s">
         <v>44</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -1971,7 +1973,7 @@
       <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="42"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="5" t="s">
         <v>39</v>
       </c>
@@ -1985,7 +1987,7 @@
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="5" t="s">
         <v>40</v>
       </c>
@@ -1999,7 +2001,7 @@
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="42"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="5" t="s">
         <v>46</v>
       </c>
@@ -2013,7 +2015,7 @@
       <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="42"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="5" t="s">
         <v>47</v>
       </c>
@@ -2027,7 +2029,7 @@
       <c r="F54" s="11"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="42"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="5" t="s">
         <v>41</v>
       </c>
@@ -2041,7 +2043,7 @@
       <c r="F55" s="11"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="42"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="5" t="s">
         <v>42</v>
       </c>
@@ -2055,7 +2057,7 @@
       <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="42"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="5" t="s">
         <v>48</v>
       </c>
@@ -2071,7 +2073,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="42"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="5" t="s">
         <v>43</v>
       </c>
@@ -2085,7 +2087,7 @@
       <c r="F58" s="11"/>
     </row>
     <row r="59" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="43"/>
+      <c r="A59" s="31"/>
       <c r="B59" s="12" t="s">
         <v>49</v>
       </c>
@@ -2101,7 +2103,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -2117,7 +2119,7 @@
       <c r="F60" s="10"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="42"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="5" t="s">
         <v>97</v>
       </c>
@@ -2131,7 +2133,7 @@
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="42"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="5" t="s">
         <v>98</v>
       </c>
@@ -2145,7 +2147,7 @@
       <c r="F62" s="11"/>
     </row>
     <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="43"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="12" t="s">
         <v>99</v>
       </c>
@@ -2159,7 +2161,7 @@
       <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="44" t="s">
+      <c r="A64" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -2175,7 +2177,7 @@
       <c r="F64" s="10"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="45"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="5" t="s">
         <v>29</v>
       </c>
@@ -2191,7 +2193,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="45"/>
+      <c r="A66" s="27"/>
       <c r="B66" s="5" t="s">
         <v>30</v>
       </c>
@@ -2207,7 +2209,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="46"/>
+      <c r="A67" s="28"/>
       <c r="B67" s="12" t="s">
         <v>31</v>
       </c>
@@ -2221,7 +2223,7 @@
       <c r="F67" s="14"/>
     </row>
     <row r="68" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="41" t="s">
+      <c r="A68" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="17" t="s">
@@ -2237,7 +2239,7 @@
       <c r="F68" s="10"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="42"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="7" t="s">
         <v>51</v>
       </c>
@@ -2251,7 +2253,7 @@
       <c r="F69" s="11"/>
     </row>
     <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A70" s="42"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="7" t="s">
         <v>52</v>
       </c>
@@ -2265,7 +2267,7 @@
       <c r="F70" s="11"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="42"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="7" t="s">
         <v>53</v>
       </c>
@@ -2279,7 +2281,7 @@
       <c r="F71" s="11"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="42"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="7" t="s">
         <v>54</v>
       </c>
@@ -2293,7 +2295,7 @@
       <c r="F72" s="11"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="42"/>
+      <c r="A73" s="30"/>
       <c r="B73" s="7" t="s">
         <v>55</v>
       </c>
@@ -2307,7 +2309,7 @@
       <c r="F73" s="11"/>
     </row>
     <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="43"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="18" t="s">
         <v>56</v>
       </c>
@@ -2321,7 +2323,7 @@
       <c r="F74" s="14"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="44" t="s">
+      <c r="A75" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B75" s="17" t="s">
@@ -2337,7 +2339,7 @@
       <c r="F75" s="10"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="45"/>
+      <c r="A76" s="27"/>
       <c r="B76" s="7" t="s">
         <v>58</v>
       </c>
@@ -2351,7 +2353,7 @@
       <c r="F76" s="11"/>
     </row>
     <row r="77" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="45"/>
+      <c r="A77" s="27"/>
       <c r="B77" s="7" t="s">
         <v>59</v>
       </c>
@@ -2365,7 +2367,7 @@
       <c r="F77" s="11"/>
     </row>
     <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A78" s="45"/>
+      <c r="A78" s="27"/>
       <c r="B78" s="7" t="s">
         <v>60</v>
       </c>
@@ -2377,7 +2379,7 @@
       <c r="F78" s="11"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="45"/>
+      <c r="A79" s="27"/>
       <c r="B79" s="7" t="s">
         <v>61</v>
       </c>
@@ -2391,7 +2393,7 @@
       <c r="F79" s="11"/>
     </row>
     <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A80" s="45"/>
+      <c r="A80" s="27"/>
       <c r="B80" s="7" t="s">
         <v>62</v>
       </c>
@@ -2405,7 +2407,7 @@
       <c r="F80" s="11"/>
     </row>
     <row r="81" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="46"/>
+      <c r="A81" s="28"/>
       <c r="B81" s="18" t="s">
         <v>63</v>
       </c>
@@ -2421,7 +2423,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="44" t="s">
+      <c r="A82" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B82" s="17" t="s">
@@ -2437,7 +2439,7 @@
       <c r="F82" s="10"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="45"/>
+      <c r="A83" s="27"/>
       <c r="B83" s="7" t="s">
         <v>68</v>
       </c>
@@ -2451,7 +2453,7 @@
       <c r="F83" s="11"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="45"/>
+      <c r="A84" s="27"/>
       <c r="B84" s="7" t="s">
         <v>69</v>
       </c>
@@ -2465,7 +2467,7 @@
       <c r="F84" s="11"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="45"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="7" t="s">
         <v>70</v>
       </c>
@@ -2479,7 +2481,7 @@
       <c r="F85" s="11"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="45"/>
+      <c r="A86" s="27"/>
       <c r="B86" s="7" t="s">
         <v>71</v>
       </c>
@@ -2493,7 +2495,7 @@
       <c r="F86" s="11"/>
     </row>
     <row r="87" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="46"/>
+      <c r="A87" s="28"/>
       <c r="B87" s="18" t="s">
         <v>72</v>
       </c>
@@ -2507,7 +2509,7 @@
       <c r="F87" s="14"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="44" t="s">
+      <c r="A88" s="26" t="s">
         <v>73</v>
       </c>
       <c r="B88" s="17" t="s">
@@ -2523,7 +2525,7 @@
       <c r="F88" s="10"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="45"/>
+      <c r="A89" s="27"/>
       <c r="B89" s="7" t="s">
         <v>75</v>
       </c>
@@ -2535,7 +2537,7 @@
       <c r="F89" s="11"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="45"/>
+      <c r="A90" s="27"/>
       <c r="B90" s="7" t="s">
         <v>76</v>
       </c>
@@ -2547,7 +2549,7 @@
       <c r="F90" s="11"/>
     </row>
     <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A91" s="45"/>
+      <c r="A91" s="27"/>
       <c r="B91" s="7" t="s">
         <v>77</v>
       </c>
@@ -2561,7 +2563,7 @@
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="46"/>
+      <c r="A92" s="28"/>
       <c r="B92" s="18" t="s">
         <v>78</v>
       </c>
@@ -2576,26 +2578,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
-    <mergeCell ref="A82:A87"/>
-    <mergeCell ref="A88:A92"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A40:A49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -2604,6 +2586,26 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="A88:A92"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:E92">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="не">

</xml_diff>

<commit_message>
add new check and toast ver-1
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK\Documents\Netology\QA\HW\Mod12_Diplom_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF2770E-6D48-4B0B-B023-2977574E3CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F91625-B139-49DC-B4E3-6DF46A20E45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="125">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -890,6 +890,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -898,60 +952,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1247,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,92 +1262,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="45">
+      <c r="B3" s="26"/>
+      <c r="C3" s="29">
         <v>45931</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="43"/>
+      <c r="B5" s="27"/>
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="40" t="s">
+      <c r="E6" s="32"/>
+      <c r="F6" s="39" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="35"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="39"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1363,7 +1363,7 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="5" t="s">
         <v>89</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="31"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="12" t="s">
         <v>90</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="44" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1431,7 +1431,7 @@
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="12" t="s">
         <v>16</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="41" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1477,7 +1477,7 @@
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="5" t="s">
         <v>84</v>
       </c>
@@ -1491,7 +1491,7 @@
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="12" t="s">
         <v>85</v>
       </c>
@@ -1505,7 +1505,7 @@
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="41" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1521,7 +1521,7 @@
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="30"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="5" t="s">
         <v>81</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="30"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="5" t="s">
         <v>86</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="12" t="s">
         <v>20</v>
       </c>
@@ -1563,7 +1563,7 @@
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="44" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1581,7 +1581,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="5" t="s">
         <v>91</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
+      <c r="A25" s="45"/>
       <c r="B25" s="5" t="s">
         <v>92</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="5" t="s">
         <v>93</v>
       </c>
@@ -1625,7 +1625,7 @@
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
+      <c r="A27" s="45"/>
       <c r="B27" s="5" t="s">
         <v>94</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
+      <c r="A28" s="45"/>
       <c r="B28" s="5" t="s">
         <v>95</v>
       </c>
@@ -1649,11 +1649,13 @@
       <c r="D28" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="12" t="s">
         <v>96</v>
       </c>
@@ -1663,11 +1665,13 @@
       <c r="D29" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="13"/>
+      <c r="E29" s="13" t="s">
+        <v>105</v>
+      </c>
       <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="44" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -1683,7 +1687,7 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="5" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1701,7 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="27"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="5" t="s">
         <v>100</v>
       </c>
@@ -1713,7 +1717,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -1721,7 +1725,7 @@
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1737,7 +1741,7 @@
       <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="30"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="23" t="s">
         <v>114</v>
       </c>
@@ -1751,7 +1755,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="5" t="s">
         <v>103</v>
       </c>
@@ -1765,7 +1769,7 @@
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="30"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="5" t="s">
         <v>101</v>
       </c>
@@ -1779,7 +1783,7 @@
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="30"/>
+      <c r="A38" s="42"/>
       <c r="B38" s="5" t="s">
         <v>102</v>
       </c>
@@ -1795,7 +1799,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="31"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="12" t="s">
         <v>104</v>
       </c>
@@ -1811,7 +1815,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="41" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -1827,7 +1831,7 @@
       <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="30"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="5" t="s">
         <v>39</v>
       </c>
@@ -1841,7 +1845,7 @@
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="30"/>
+      <c r="A42" s="42"/>
       <c r="B42" s="5" t="s">
         <v>40</v>
       </c>
@@ -1855,7 +1859,7 @@
       <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="30"/>
+      <c r="A43" s="42"/>
       <c r="B43" s="5" t="s">
         <v>121</v>
       </c>
@@ -1869,7 +1873,7 @@
       <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
+      <c r="A44" s="42"/>
       <c r="B44" s="5" t="s">
         <v>122</v>
       </c>
@@ -1883,7 +1887,7 @@
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="5" t="s">
         <v>41</v>
       </c>
@@ -1897,7 +1901,7 @@
       <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="5" t="s">
         <v>42</v>
       </c>
@@ -1911,7 +1915,7 @@
       <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="30"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="5" t="s">
         <v>123</v>
       </c>
@@ -1927,7 +1931,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="30"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="5" t="s">
         <v>43</v>
       </c>
@@ -1941,7 +1945,7 @@
       <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="31"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="12" t="s">
         <v>124</v>
       </c>
@@ -1957,7 +1961,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="41" t="s">
         <v>44</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -1973,7 +1977,7 @@
       <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="30"/>
+      <c r="A51" s="42"/>
       <c r="B51" s="5" t="s">
         <v>39</v>
       </c>
@@ -1987,7 +1991,7 @@
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="30"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="5" t="s">
         <v>40</v>
       </c>
@@ -2001,7 +2005,7 @@
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="30"/>
+      <c r="A53" s="42"/>
       <c r="B53" s="5" t="s">
         <v>46</v>
       </c>
@@ -2015,7 +2019,7 @@
       <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
+      <c r="A54" s="42"/>
       <c r="B54" s="5" t="s">
         <v>47</v>
       </c>
@@ -2029,7 +2033,7 @@
       <c r="F54" s="11"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="30"/>
+      <c r="A55" s="42"/>
       <c r="B55" s="5" t="s">
         <v>41</v>
       </c>
@@ -2043,7 +2047,7 @@
       <c r="F55" s="11"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
+      <c r="A56" s="42"/>
       <c r="B56" s="5" t="s">
         <v>42</v>
       </c>
@@ -2057,7 +2061,7 @@
       <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="30"/>
+      <c r="A57" s="42"/>
       <c r="B57" s="5" t="s">
         <v>48</v>
       </c>
@@ -2073,7 +2077,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="30"/>
+      <c r="A58" s="42"/>
       <c r="B58" s="5" t="s">
         <v>43</v>
       </c>
@@ -2087,7 +2091,7 @@
       <c r="F58" s="11"/>
     </row>
     <row r="59" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="31"/>
+      <c r="A59" s="43"/>
       <c r="B59" s="12" t="s">
         <v>49</v>
       </c>
@@ -2103,7 +2107,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="41" t="s">
         <v>26</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -2119,7 +2123,7 @@
       <c r="F60" s="10"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="30"/>
+      <c r="A61" s="42"/>
       <c r="B61" s="5" t="s">
         <v>97</v>
       </c>
@@ -2133,7 +2137,7 @@
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="30"/>
+      <c r="A62" s="42"/>
       <c r="B62" s="5" t="s">
         <v>98</v>
       </c>
@@ -2147,7 +2151,7 @@
       <c r="F62" s="11"/>
     </row>
     <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="31"/>
+      <c r="A63" s="43"/>
       <c r="B63" s="12" t="s">
         <v>99</v>
       </c>
@@ -2161,7 +2165,7 @@
       <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="26" t="s">
+      <c r="A64" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -2177,7 +2181,7 @@
       <c r="F64" s="10"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="27"/>
+      <c r="A65" s="45"/>
       <c r="B65" s="5" t="s">
         <v>29</v>
       </c>
@@ -2193,7 +2197,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="27"/>
+      <c r="A66" s="45"/>
       <c r="B66" s="5" t="s">
         <v>30</v>
       </c>
@@ -2209,7 +2213,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="28"/>
+      <c r="A67" s="46"/>
       <c r="B67" s="12" t="s">
         <v>31</v>
       </c>
@@ -2223,7 +2227,7 @@
       <c r="F67" s="14"/>
     </row>
     <row r="68" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="41" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="17" t="s">
@@ -2239,7 +2243,7 @@
       <c r="F68" s="10"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="30"/>
+      <c r="A69" s="42"/>
       <c r="B69" s="7" t="s">
         <v>51</v>
       </c>
@@ -2253,7 +2257,7 @@
       <c r="F69" s="11"/>
     </row>
     <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A70" s="30"/>
+      <c r="A70" s="42"/>
       <c r="B70" s="7" t="s">
         <v>52</v>
       </c>
@@ -2267,7 +2271,7 @@
       <c r="F70" s="11"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="30"/>
+      <c r="A71" s="42"/>
       <c r="B71" s="7" t="s">
         <v>53</v>
       </c>
@@ -2281,7 +2285,7 @@
       <c r="F71" s="11"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="30"/>
+      <c r="A72" s="42"/>
       <c r="B72" s="7" t="s">
         <v>54</v>
       </c>
@@ -2295,7 +2299,7 @@
       <c r="F72" s="11"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="30"/>
+      <c r="A73" s="42"/>
       <c r="B73" s="7" t="s">
         <v>55</v>
       </c>
@@ -2309,7 +2313,7 @@
       <c r="F73" s="11"/>
     </row>
     <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="31"/>
+      <c r="A74" s="43"/>
       <c r="B74" s="18" t="s">
         <v>56</v>
       </c>
@@ -2323,7 +2327,7 @@
       <c r="F74" s="14"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="26" t="s">
+      <c r="A75" s="44" t="s">
         <v>57</v>
       </c>
       <c r="B75" s="17" t="s">
@@ -2339,7 +2343,7 @@
       <c r="F75" s="10"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="27"/>
+      <c r="A76" s="45"/>
       <c r="B76" s="7" t="s">
         <v>58</v>
       </c>
@@ -2353,7 +2357,7 @@
       <c r="F76" s="11"/>
     </row>
     <row r="77" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="27"/>
+      <c r="A77" s="45"/>
       <c r="B77" s="7" t="s">
         <v>59</v>
       </c>
@@ -2367,7 +2371,7 @@
       <c r="F77" s="11"/>
     </row>
     <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A78" s="27"/>
+      <c r="A78" s="45"/>
       <c r="B78" s="7" t="s">
         <v>60</v>
       </c>
@@ -2379,7 +2383,7 @@
       <c r="F78" s="11"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="27"/>
+      <c r="A79" s="45"/>
       <c r="B79" s="7" t="s">
         <v>61</v>
       </c>
@@ -2393,7 +2397,7 @@
       <c r="F79" s="11"/>
     </row>
     <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A80" s="27"/>
+      <c r="A80" s="45"/>
       <c r="B80" s="7" t="s">
         <v>62</v>
       </c>
@@ -2407,7 +2411,7 @@
       <c r="F80" s="11"/>
     </row>
     <row r="81" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="28"/>
+      <c r="A81" s="46"/>
       <c r="B81" s="18" t="s">
         <v>63</v>
       </c>
@@ -2423,7 +2427,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="26" t="s">
+      <c r="A82" s="44" t="s">
         <v>65</v>
       </c>
       <c r="B82" s="17" t="s">
@@ -2439,7 +2443,7 @@
       <c r="F82" s="10"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="27"/>
+      <c r="A83" s="45"/>
       <c r="B83" s="7" t="s">
         <v>68</v>
       </c>
@@ -2453,7 +2457,7 @@
       <c r="F83" s="11"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="27"/>
+      <c r="A84" s="45"/>
       <c r="B84" s="7" t="s">
         <v>69</v>
       </c>
@@ -2467,7 +2471,7 @@
       <c r="F84" s="11"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="27"/>
+      <c r="A85" s="45"/>
       <c r="B85" s="7" t="s">
         <v>70</v>
       </c>
@@ -2481,7 +2485,7 @@
       <c r="F85" s="11"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="27"/>
+      <c r="A86" s="45"/>
       <c r="B86" s="7" t="s">
         <v>71</v>
       </c>
@@ -2495,7 +2499,7 @@
       <c r="F86" s="11"/>
     </row>
     <row r="87" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="28"/>
+      <c r="A87" s="46"/>
       <c r="B87" s="18" t="s">
         <v>72</v>
       </c>
@@ -2509,7 +2513,7 @@
       <c r="F87" s="14"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="44" t="s">
         <v>73</v>
       </c>
       <c r="B88" s="17" t="s">
@@ -2525,7 +2529,7 @@
       <c r="F88" s="10"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="27"/>
+      <c r="A89" s="45"/>
       <c r="B89" s="7" t="s">
         <v>75</v>
       </c>
@@ -2537,7 +2541,7 @@
       <c r="F89" s="11"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="27"/>
+      <c r="A90" s="45"/>
       <c r="B90" s="7" t="s">
         <v>76</v>
       </c>
@@ -2549,7 +2553,7 @@
       <c r="F90" s="11"/>
     </row>
     <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A91" s="27"/>
+      <c r="A91" s="45"/>
       <c r="B91" s="7" t="s">
         <v>77</v>
       </c>
@@ -2563,7 +2567,7 @@
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="28"/>
+      <c r="A92" s="46"/>
       <c r="B92" s="18" t="s">
         <v>78</v>
       </c>
@@ -2578,6 +2582,26 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="A88:A92"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -2586,26 +2610,6 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A40:A49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
-    <mergeCell ref="A82:A87"/>
-    <mergeCell ref="A88:A92"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:E92">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="не">

</xml_diff>